<commit_message>
changes from Monday meeting
</commit_message>
<xml_diff>
--- a/morphological matrix/Master Morphological Matrix.xlsx
+++ b/morphological matrix/Master Morphological Matrix.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="48">
   <si>
     <t>Payload Package</t>
   </si>
@@ -65,9 +65,30 @@
     <t>DSI-EUVI-MAG</t>
   </si>
   <si>
+    <t>same</t>
+  </si>
+  <si>
     <t>Second Stage Propulsion</t>
   </si>
   <si>
+    <t>Cost $ 1</t>
+  </si>
+  <si>
+    <t>Cost $ 2</t>
+  </si>
+  <si>
+    <t>Cost $ 3</t>
+  </si>
+  <si>
+    <t>Mission Value 1</t>
+  </si>
+  <si>
+    <t>Mission Value 2</t>
+  </si>
+  <si>
+    <t>Mission Value 3</t>
+  </si>
+  <si>
     <t>Solar Sail</t>
   </si>
   <si>
@@ -80,6 +101,9 @@
     <t>Nuclear</t>
   </si>
   <si>
+    <t>Mission Value Functions if not neglected:</t>
+  </si>
+  <si>
     <t>Lift-Off Systems</t>
   </si>
   <si>
@@ -92,12 +116,6 @@
     <t>SpaceX Starship</t>
   </si>
   <si>
-    <t>ULA Atlas V 551</t>
-  </si>
-  <si>
-    <t>ULA Delta IV Heavy</t>
-  </si>
-  <si>
     <t>ULA Vulcan Centaur Heavy</t>
   </si>
   <si>
@@ -107,18 +125,6 @@
     <t>Inclination Change Method</t>
   </si>
   <si>
-    <t>Reliability</t>
-  </si>
-  <si>
-    <t>Monetary Cost</t>
-  </si>
-  <si>
-    <t>Mission Value</t>
-  </si>
-  <si>
-    <t>Direct Transfer from 1 AU</t>
-  </si>
-  <si>
     <t>Bielliptic Transfer</t>
   </si>
   <si>
@@ -153,9 +159,6 @@
   </si>
   <si>
     <t>POLARIS Final Orbit</t>
-  </si>
-  <si>
-    <t>same as 2</t>
   </si>
 </sst>
 </file>
@@ -195,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -208,6 +211,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -217,11 +223,19 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -265,13 +279,23 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="5">
+  <tableStyles count="7">
     <tableStyle count="3" pivot="0" name="Payload Package-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="Second Stage Propulsion-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Second Stage Propulsion-style 2">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Second Stage Propulsion-style 3">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -316,7 +340,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A2:K6" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A2:K7" displayName="Table_1" id="1">
   <tableColumns count="11">
     <tableColumn name="ID" id="1"/>
     <tableColumn name="Option" id="2"/>
@@ -335,7 +359,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A2:K6" displayName="Table_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A2:K7" displayName="Table_2" id="2">
   <tableColumns count="11">
     <tableColumn name="ID" id="1"/>
     <tableColumn name="Option" id="2"/>
@@ -354,7 +378,27 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A2:K9" displayName="Table_3" id="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="I11:K15" displayName="Table_3" id="3">
+  <tableColumns count="3">
+    <tableColumn name="Value 1" id="1"/>
+    <tableColumn name="Value 2" id="2"/>
+    <tableColumn name="Value 3" id="3"/>
+  </tableColumns>
+  <tableStyleInfo name="Second Stage Propulsion-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="H11:H15" displayName="Table_4" id="4">
+  <tableColumns count="1">
+    <tableColumn name="Option" id="1"/>
+  </tableColumns>
+  <tableStyleInfo name="Second Stage Propulsion-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A2:K8" displayName="Table_5" id="5">
   <tableColumns count="11">
     <tableColumn name="ID" id="1"/>
     <tableColumn name="Option" id="2"/>
@@ -372,8 +416,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A2:K8" displayName="Table_4" id="4">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A2:K8" displayName="Table_6" id="6">
   <tableColumns count="11">
     <tableColumn name="ID" id="1"/>
     <tableColumn name="Option" id="2"/>
@@ -391,8 +435,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A2:K9" displayName="Table_5" id="5">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A2:K9" displayName="Table_7" id="7">
   <tableColumns count="11">
     <tableColumn name="ID" id="1"/>
     <tableColumn name="Option" id="2"/>
@@ -805,57 +849,81 @@
         <v>0.5996978851963747</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
     <row r="10">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-    </row>
-    <row r="11">
-      <c r="C11" s="8"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12">
-      <c r="C12" s="8"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13">
-      <c r="C13" s="8"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14">
-      <c r="C14" s="8"/>
-      <c r="I14" s="9"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
     </row>
     <row r="15">
-      <c r="C15" s="8"/>
-      <c r="I15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16">
-      <c r="C16" s="8"/>
-      <c r="I16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="I16" s="10"/>
     </row>
     <row r="17">
-      <c r="C17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
       <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
     </row>
     <row r="18">
-      <c r="C18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
       <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
     </row>
     <row r="19">
-      <c r="C19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
       <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+    </row>
+    <row r="20">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -883,8 +951,8 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="s">
-        <v>16</v>
+      <c r="A1" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2">
@@ -921,40 +989,94 @@
       <c r="K2" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="M2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4">
         <v>4.1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0.9999999999999999</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H3" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0.9999999999999999</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0.9999999999999999</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0.9999999999999999</v>
+        <v>24</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="G3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="H3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="I3" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="K3" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="M3" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="N3" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="O3" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="P3" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="Q3" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="R3" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="S3" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="T3" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="U3" s="12">
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -962,34 +1084,61 @@
         <v>4.2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1.0200001141552513</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1.1478573140900197</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.4935714856490541</v>
-      </c>
-      <c r="F4" s="5">
-        <v>4.968490878938639</v>
-      </c>
-      <c r="G4" s="5">
-        <v>3.4779436152570473</v>
-      </c>
-      <c r="H4" s="5">
-        <v>4.968490878938639</v>
-      </c>
-      <c r="I4" s="5">
-        <v>1.1552126721749365</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0.7838895102803901</v>
-      </c>
-      <c r="K4" s="5">
-        <v>1.2336344754696784</v>
+        <v>25</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1.02</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1.148</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.494</v>
+      </c>
+      <c r="F4" s="13">
+        <v>4.968</v>
+      </c>
+      <c r="G4" s="13">
+        <v>4.968</v>
+      </c>
+      <c r="H4" s="13">
+        <v>4.968</v>
+      </c>
+      <c r="I4" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="M4" s="12">
+        <v>1.02</v>
+      </c>
+      <c r="N4" s="12">
+        <v>1.148</v>
+      </c>
+      <c r="O4" s="12">
+        <v>0.494</v>
+      </c>
+      <c r="P4" s="12">
+        <v>4.968</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>3.478</v>
+      </c>
+      <c r="R4" s="12">
+        <v>4.968</v>
+      </c>
+      <c r="S4" s="12">
+        <v>1.373477643</v>
+      </c>
+      <c r="T4" s="12">
+        <v>0.8198208344</v>
+      </c>
+      <c r="U4" s="12">
+        <v>1.30338766</v>
       </c>
     </row>
     <row r="5">
@@ -997,34 +1146,61 @@
         <v>4.3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0.9650000000000001</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1.0617857142857146</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.645357142857143</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0.16417910447761191</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0.14365671641791042</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0.16417910447761191</v>
-      </c>
-      <c r="I5" s="5">
-        <v>1.5880439470974368</v>
-      </c>
-      <c r="J5" s="5">
-        <v>1.4429368710169763</v>
-      </c>
-      <c r="K5" s="5">
-        <v>2.0138457085374313</v>
+        <v>26</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0.965</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1.062</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.645</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.752</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0.752</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0.752</v>
+      </c>
+      <c r="I5" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="K5" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="M5" s="12">
+        <v>0.965</v>
+      </c>
+      <c r="N5" s="12">
+        <v>1.062</v>
+      </c>
+      <c r="O5" s="12">
+        <v>0.645</v>
+      </c>
+      <c r="P5" s="12">
+        <v>0.682</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>0.597</v>
+      </c>
+      <c r="R5" s="12">
+        <v>0.682</v>
+      </c>
+      <c r="S5" s="12">
+        <v>1.127633498</v>
+      </c>
+      <c r="T5" s="12">
+        <v>0.985823317</v>
+      </c>
+      <c r="U5" s="12">
+        <v>1.003045156</v>
       </c>
     </row>
     <row r="6">
@@ -1032,34 +1208,151 @@
         <v>4.4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0.11000228310502284</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.11678913894324856</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.0753582844096543</v>
-      </c>
-      <c r="F6" s="5">
-        <v>7.553344389165283</v>
-      </c>
-      <c r="G6" s="5">
-        <v>52.873410724156976</v>
-      </c>
-      <c r="H6" s="5">
-        <v>7.553344389165283</v>
-      </c>
-      <c r="I6" s="5">
-        <v>1.0687343940304113</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0.03954689844760136</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0.14925156015391125</v>
+        <v>27</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.11</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.117</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.075</v>
+      </c>
+      <c r="F6" s="13">
+        <v>7.553</v>
+      </c>
+      <c r="G6" s="13">
+        <v>7.553</v>
+      </c>
+      <c r="H6" s="13">
+        <v>7.553</v>
+      </c>
+      <c r="I6" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="K6" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="M6" s="12">
+        <v>0.11</v>
+      </c>
+      <c r="N6" s="12">
+        <v>0.117</v>
+      </c>
+      <c r="O6" s="12">
+        <v>0.075</v>
+      </c>
+      <c r="P6" s="12">
+        <v>7.553</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>52.873</v>
+      </c>
+      <c r="R6" s="12">
+        <v>7.553</v>
+      </c>
+      <c r="S6" s="12">
+        <v>1.346757863</v>
+      </c>
+      <c r="T6" s="12">
+        <v>0.3534146269</v>
+      </c>
+      <c r="U6" s="12">
+        <v>1.483457185</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="11">
+      <c r="G11" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="H12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="J12" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="K12" s="13">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="H13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="13">
+        <v>1.3735</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0.8198</v>
+      </c>
+      <c r="K13" s="13">
+        <v>1.3034</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="H14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="13">
+        <v>1.1276</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0.9858</v>
+      </c>
+      <c r="K14" s="13">
+        <v>1.003</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="H15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="13">
+        <v>1.3468</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0.3534</v>
+      </c>
+      <c r="K15" s="13">
+        <v>1.4835</v>
       </c>
     </row>
   </sheetData>
@@ -1067,8 +1360,10 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1088,8 +1383,8 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="s">
-        <v>21</v>
+      <c r="A1" s="11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2">
@@ -1132,34 +1427,34 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0.3522554274768786</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0.3522554274768786</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.3522554274768786</v>
-      </c>
-      <c r="F3" s="5">
-        <v>25.0</v>
-      </c>
-      <c r="G3" s="5">
-        <v>25.0</v>
-      </c>
-      <c r="H3" s="5">
-        <v>25.0</v>
-      </c>
-      <c r="I3" s="5">
-        <v>2.5338576498913525</v>
-      </c>
-      <c r="J3" s="5">
-        <v>4.056643397454103</v>
-      </c>
-      <c r="K3" s="5">
-        <v>6.598344829071966</v>
+        <v>30</v>
+      </c>
+      <c r="C3" s="13">
+        <v>0.352</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0.633</v>
+      </c>
+      <c r="E3" s="13">
+        <v>0.937</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="I3" s="13">
+        <v>5.99</v>
+      </c>
+      <c r="J3" s="13">
+        <v>4.057</v>
+      </c>
+      <c r="K3" s="13">
+        <v>6.598</v>
       </c>
     </row>
     <row r="4">
@@ -1167,34 +1462,34 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.5643343270888359</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.5643343270888359</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.5643343270888359</v>
-      </c>
-      <c r="F4" s="5">
-        <v>1.125</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1.125</v>
-      </c>
-      <c r="H4" s="5">
-        <v>1.125</v>
-      </c>
-      <c r="I4" s="5">
-        <v>2.312386218459863</v>
-      </c>
-      <c r="J4" s="5">
-        <v>3.429817443349683</v>
-      </c>
-      <c r="K4" s="5">
-        <v>5.02500650069466</v>
+        <v>31</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0.564</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0.901</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.991</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="I4" s="13">
+        <v>4.12</v>
+      </c>
+      <c r="J4" s="13">
+        <v>3.43</v>
+      </c>
+      <c r="K4" s="13">
+        <v>5.025</v>
       </c>
     </row>
     <row r="5">
@@ -1202,175 +1497,128 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0.3522554274768786</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.3522554274768786</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.3522554274768786</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0.125</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0.125</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0.125</v>
-      </c>
-      <c r="I5" s="5">
-        <v>4.86384509665026</v>
-      </c>
-      <c r="J5" s="5">
-        <v>13.339730733818561</v>
-      </c>
-      <c r="K5" s="5">
-        <v>19.128058437930324</v>
+        <v>32</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0.352</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.633</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.998</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="I5" s="13">
+        <v>14.22</v>
+      </c>
+      <c r="J5" s="13">
+        <v>13.34</v>
+      </c>
+      <c r="K5" s="13">
+        <v>19.128</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0.7446480192287507</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.7446480192287507</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.7446480192287507</v>
-      </c>
-      <c r="F6" s="5">
-        <v>1.3625</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1.3625</v>
-      </c>
-      <c r="H6" s="5">
-        <v>1.3625</v>
-      </c>
-      <c r="I6" s="5">
-        <v>1.0460522641900651</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0.9157736447579272</v>
-      </c>
-      <c r="K6" s="5">
-        <v>1.0053875580437464</v>
+        <v>33</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.352</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.633</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.993</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="I6" s="13">
+        <v>2.13</v>
+      </c>
+      <c r="J6" s="13">
+        <v>2.31</v>
+      </c>
+      <c r="K6" s="13">
+        <v>2.278</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0.7559852486279516</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0.7559852486279516</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0.7559852486279516</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1.8625</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1.8625</v>
-      </c>
-      <c r="H7" s="5">
-        <v>1.8625</v>
-      </c>
-      <c r="I7" s="5">
-        <v>1.1339060585874143</v>
-      </c>
-      <c r="J7" s="5">
-        <v>1.0518025221621576</v>
-      </c>
-      <c r="K7" s="5">
-        <v>1.3760734763132334</v>
+        <v>34</v>
+      </c>
+      <c r="C7" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="I7" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="J7" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="K7" s="13">
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.3522554274768786</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.3522554274768786</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.3522554274768786</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1.25</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1.25</v>
-      </c>
-      <c r="H8" s="5">
-        <v>1.25</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0.7320832252204684</v>
-      </c>
-      <c r="J8" s="5">
-        <v>2.309547358252985</v>
-      </c>
-      <c r="K8" s="5">
-        <v>2.278159777296862</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4">
-        <v>7.0</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H9" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I9" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="J9" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="K9" s="5">
-        <v>1.0</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1404,7 +1652,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
@@ -1441,226 +1689,118 @@
       <c r="K2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="4">
-        <v>8.1</v>
+        <v>8.2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C3" s="5">
-        <v>0.012499999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="D3" s="5">
-        <v>0.012499999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="E3" s="5">
-        <v>0.012499999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="F3" s="5">
-        <v>74.80897668038409</v>
+        <v>6.087395555555556</v>
       </c>
       <c r="G3" s="5">
-        <v>73.04181980562122</v>
+        <v>6.79799829787234</v>
       </c>
       <c r="H3" s="5">
-        <v>76.74052024117141</v>
+        <v>5.31069023255814</v>
       </c>
       <c r="I3" s="5">
-        <v>1.3636195752539244</v>
+        <v>0.45453985841797473</v>
       </c>
       <c r="J3" s="5">
-        <v>3.511076303423585</v>
+        <v>1.1703587678078615</v>
       </c>
       <c r="K3" s="5">
-        <v>1.8624963966560968</v>
-      </c>
-      <c r="M3" s="11">
-        <v>0.012499999999999999</v>
-      </c>
-      <c r="N3" s="11">
-        <v>0.012499999999999999</v>
-      </c>
-      <c r="O3" s="11">
-        <v>0.012499999999999999</v>
-      </c>
-      <c r="P3" s="11">
-        <v>74.80897668038409</v>
-      </c>
-      <c r="Q3" s="11">
-        <v>73.04181980562122</v>
-      </c>
-      <c r="R3" s="11">
-        <v>76.74052024117141</v>
-      </c>
-      <c r="S3" s="11">
-        <v>1.3636195752539244</v>
-      </c>
-      <c r="T3" s="11">
-        <v>3.511076303423585</v>
-      </c>
-      <c r="U3" s="11">
-        <v>1.8624963966560968</v>
+        <v>0.6208321322186989</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4">
-        <v>8.2</v>
+        <v>8.3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C4" s="5">
-        <v>0.25</v>
+        <v>0.8749999999999999</v>
       </c>
       <c r="D4" s="5">
-        <v>0.25</v>
+        <v>0.8749999999999999</v>
       </c>
       <c r="E4" s="5">
-        <v>0.25</v>
+        <v>0.8749999999999999</v>
       </c>
       <c r="F4" s="5">
-        <v>6.087395555555556</v>
+        <v>1.015873015873016</v>
       </c>
       <c r="G4" s="5">
-        <v>6.79799829787234</v>
+        <v>0.9726443768996962</v>
       </c>
       <c r="H4" s="5">
-        <v>5.31069023255814</v>
+        <v>1.0631229235880402</v>
       </c>
       <c r="I4" s="5">
-        <v>0.45453985841797473</v>
+        <v>0.9943059402893198</v>
       </c>
       <c r="J4" s="5">
-        <v>1.1703587678078615</v>
+        <v>0.9853388155441187</v>
       </c>
       <c r="K4" s="5">
-        <v>0.6208321322186989</v>
-      </c>
-      <c r="M4" s="11">
-        <v>0.25</v>
-      </c>
-      <c r="N4" s="11">
-        <v>0.25</v>
-      </c>
-      <c r="O4" s="11">
-        <v>0.25</v>
-      </c>
-      <c r="P4" s="11">
-        <v>6.087395555555556</v>
-      </c>
-      <c r="Q4" s="11">
-        <v>6.79799829787234</v>
-      </c>
-      <c r="R4" s="11">
-        <v>5.31069023255814</v>
-      </c>
-      <c r="S4" s="11">
-        <v>0.45453985841797473</v>
-      </c>
-      <c r="T4" s="11">
-        <v>1.1703587678078615</v>
-      </c>
-      <c r="U4" s="11">
-        <v>0.6208321322186989</v>
+        <v>0.992222782742385</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4">
-        <v>8.3</v>
+        <v>8.4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C5" s="5">
-        <v>0.8749999999999999</v>
+        <v>1.125</v>
       </c>
       <c r="D5" s="5">
-        <v>0.8749999999999999</v>
+        <v>1.125</v>
       </c>
       <c r="E5" s="5">
-        <v>0.8749999999999999</v>
+        <v>1.125</v>
       </c>
       <c r="F5" s="5">
-        <v>1.015873015873016</v>
+        <v>1.2084241103848947</v>
       </c>
       <c r="G5" s="5">
-        <v>0.9726443768996962</v>
+        <v>1.3172020581282156</v>
       </c>
       <c r="H5" s="5">
-        <v>1.0631229235880402</v>
+        <v>1.0895272837817296</v>
       </c>
       <c r="I5" s="5">
-        <v>0.9943059402893198</v>
+        <v>1.0340781779008925</v>
       </c>
       <c r="J5" s="5">
-        <v>0.9853388155441187</v>
+        <v>1.0877452077273067</v>
       </c>
       <c r="K5" s="5">
-        <v>0.992222782742385</v>
-      </c>
-      <c r="M5" s="11">
-        <v>0.8749999999999999</v>
-      </c>
-      <c r="N5" s="11">
-        <v>0.8749999999999999</v>
-      </c>
-      <c r="O5" s="11">
-        <v>0.8749999999999999</v>
-      </c>
-      <c r="P5" s="11">
-        <v>1.015873015873016</v>
-      </c>
-      <c r="Q5" s="11">
-        <v>0.9726443768996962</v>
-      </c>
-      <c r="R5" s="11">
-        <v>1.0631229235880402</v>
-      </c>
-      <c r="S5" s="11">
-        <v>0.9943059402893198</v>
-      </c>
-      <c r="T5" s="11">
-        <v>0.9853388155441187</v>
-      </c>
-      <c r="U5" s="11">
-        <v>0.992222782742385</v>
+        <v>1.0465455943115212</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4">
-        <v>8.4</v>
+        <v>8.5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C6" s="5">
         <v>1.125</v>
@@ -1672,174 +1812,75 @@
         <v>1.125</v>
       </c>
       <c r="F6" s="5">
-        <v>1.2084241103848947</v>
+        <v>1.158228031953522</v>
       </c>
       <c r="G6" s="5">
-        <v>1.3172020581282156</v>
+        <v>1.2499179529968014</v>
       </c>
       <c r="H6" s="5">
-        <v>1.0895272837817296</v>
+        <v>1.0580088159294727</v>
       </c>
       <c r="I6" s="5">
-        <v>1.0340781779008925</v>
+        <v>1.062049861495845</v>
       </c>
       <c r="J6" s="5">
-        <v>1.0877452077273067</v>
+        <v>1.159767285746252</v>
       </c>
       <c r="K6" s="5">
-        <v>1.0465455943115212</v>
-      </c>
-      <c r="M6" s="11">
-        <v>1.125</v>
-      </c>
-      <c r="N6" s="11">
-        <v>1.125</v>
-      </c>
-      <c r="O6" s="11">
-        <v>1.125</v>
-      </c>
-      <c r="P6" s="11">
-        <v>1.2084241103848947</v>
-      </c>
-      <c r="Q6" s="11">
-        <v>1.3172020581282156</v>
-      </c>
-      <c r="R6" s="11">
-        <v>1.0895272837817296</v>
-      </c>
-      <c r="S6" s="11">
-        <v>1.0340781779008925</v>
-      </c>
-      <c r="T6" s="11">
-        <v>1.0877452077273067</v>
-      </c>
-      <c r="U6" s="11">
-        <v>1.0465455943115212</v>
+        <v>1.0847506486019025</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C7" s="5">
-        <v>1.125</v>
+        <v>1.0</v>
       </c>
       <c r="D7" s="5">
-        <v>1.125</v>
+        <v>1.0</v>
       </c>
       <c r="E7" s="5">
-        <v>1.125</v>
+        <v>1.0</v>
       </c>
       <c r="F7" s="5">
-        <v>1.158228031953522</v>
+        <v>1.0</v>
       </c>
       <c r="G7" s="5">
-        <v>1.2499179529968014</v>
+        <v>1.0</v>
       </c>
       <c r="H7" s="5">
-        <v>1.0580088159294727</v>
+        <v>1.0</v>
       </c>
       <c r="I7" s="5">
-        <v>1.062049861495845</v>
+        <v>1.0</v>
       </c>
       <c r="J7" s="5">
-        <v>1.159767285746252</v>
+        <v>1.0</v>
       </c>
       <c r="K7" s="5">
-        <v>1.0847506486019025</v>
-      </c>
-      <c r="M7" s="11">
-        <v>1.125</v>
-      </c>
-      <c r="N7" s="11">
-        <v>1.125</v>
-      </c>
-      <c r="O7" s="11">
-        <v>1.125</v>
-      </c>
-      <c r="P7" s="11">
-        <v>1.158228031953522</v>
-      </c>
-      <c r="Q7" s="11">
-        <v>1.2499179529968014</v>
-      </c>
-      <c r="R7" s="11">
-        <v>1.0580088159294727</v>
-      </c>
-      <c r="S7" s="11">
-        <v>1.062049861495845</v>
-      </c>
-      <c r="T7" s="11">
-        <v>1.159767285746252</v>
-      </c>
-      <c r="U7" s="11">
-        <v>1.0847506486019025</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4">
-        <v>8.6</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I8" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="J8" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="K8" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="M8" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="N8" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="O8" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="P8" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="Q8" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="R8" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="S8" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="T8" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="U8" s="11">
-        <v>1.0</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1869,7 +1910,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1922,33 +1963,33 @@
         <v>5.1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="12">
+        <v>41</v>
+      </c>
+      <c r="C3" s="16">
         <v>1.2142857142857144</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="16">
         <v>1.2142857142857144</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="16">
         <v>1.2142857142857144</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="16">
         <v>0.9189189189189189</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="16">
         <v>0.9641434262948207</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="16">
         <v>0.9641434262948207</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="16">
         <v>1.6203885263203632</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="16">
         <v>1.5107219133322252</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="16">
         <v>1.5107219133322252</v>
       </c>
     </row>
@@ -1957,33 +1998,33 @@
         <v>5.2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="12">
+        <v>42</v>
+      </c>
+      <c r="C4" s="16">
         <v>1.142857142857143</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="16">
         <v>1.142857142857143</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="16">
         <v>1.142857142857143</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="16">
         <v>3.292063492063491</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="16">
         <v>3.1367741935483866</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="16">
         <v>3.1367741935483866</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="16">
         <v>1.4811535033045609</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="16">
         <v>1.3535587183538316</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="16">
         <v>1.3535587183538316</v>
       </c>
     </row>
@@ -1992,33 +2033,33 @@
         <v>5.3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="12">
+        <v>43</v>
+      </c>
+      <c r="C5" s="16">
         <v>1.142857142857143</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="16">
         <v>1.142857142857143</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="16">
         <v>1.142857142857143</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="16">
         <v>1.0523809523809522</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="16">
         <v>1.0751612903225805</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="16">
         <v>1.0751612903225805</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="16">
         <v>1.252119860223303</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="16">
         <v>1.1267141438343644</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="16">
         <v>1.1267141438343644</v>
       </c>
     </row>
@@ -2027,33 +2068,33 @@
         <v>5.4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="D6" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="F6" s="12">
+        <v>44</v>
+      </c>
+      <c r="C6" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="F6" s="16">
         <v>2.8000000000000003</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="16">
         <v>2.6036363636363635</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="16">
         <v>2.6036363636363635</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="16">
         <v>0.3843160366952889</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="16">
         <v>0.3644097465686298</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="16">
         <v>0.3644097465686298</v>
       </c>
     </row>
@@ -2062,33 +2103,33 @@
         <v>5.5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="12">
+        <v>45</v>
+      </c>
+      <c r="C7" s="16">
         <v>1.2857142857142858</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="16">
         <v>1.2857142857142858</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="16">
         <v>1.2857142857142858</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="16">
         <v>0.25563909774436083</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="16">
         <v>0.34645669291338577</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="16">
         <v>0.34645669291338577</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="16">
         <v>1.1261472319933628</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="16">
         <v>1.1294188714495659</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="16">
         <v>1.1294188714495659</v>
       </c>
     </row>
@@ -2097,33 +2138,33 @@
         <v>5.6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="12">
+        <v>46</v>
+      </c>
+      <c r="C8" s="16">
         <v>0.7142857142857143</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="16">
         <v>0.7142857142857143</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="16">
         <v>0.7142857142857143</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="16">
         <v>0.32380952380952377</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="16">
         <v>0.3826086956521739</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="16">
         <v>0.3826086956521739</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="16">
         <v>0.9479392241523262</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="16">
         <v>0.8923739692585146</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="16">
         <v>0.8923739692585146</v>
       </c>
     </row>
@@ -2132,45 +2173,34 @@
         <v>5.7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="F9" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="G9" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="H9" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="I9" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="J9" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="K9" s="12">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="E11" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="C9" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="F9" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="H9" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="I9" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="J9" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="K9" s="16">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>